<commit_message>
Committing before I rename some files
</commit_message>
<xml_diff>
--- a/files-to-read/test_spreadsheet.xlsx
+++ b/files-to-read/test_spreadsheet.xlsx
@@ -106,6 +106,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -123,18 +124,12 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6E0EC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -176,7 +171,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -189,66 +184,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFE6E0EC"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -260,7 +195,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1:H4"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>